<commit_message>
Reorganize and enhance instrumentation configuration.
Reordered and added missing entries in `instruments_tree.json`. This includes adjustments in the hierarchy and expanded configurations for various instruments (e.g., `JMS DX-300`, `JMS-T100LP`). Ensured consistency across definitions and improved clarity in the nested structure.
</commit_message>
<xml_diff>
--- a/Instrument_tree.xlsx
+++ b/Instrument_tree.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Axel\PYTHON\FragHub\TOOLS\generate_decision_tree\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Axel\PYTHON\FragHub\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7486495A-1618-41D4-854C-234BEA5E1D9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4424CCA-3681-4334-B804-964964755BF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-285" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AB SCIEX" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1836" uniqueCount="327">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1842" uniqueCount="328">
   <si>
     <t>MARQUES</t>
   </si>
@@ -1009,6 +1009,9 @@
   </si>
   <si>
     <t>GC Orbitrap Q-Exactive</t>
+  </si>
+  <si>
+    <t>JMS-700V</t>
   </si>
 </sst>
 </file>
@@ -2602,10 +2605,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2856,6 +2859,26 @@
       </c>
       <c r="F12" t="s">
         <v>35</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>79</v>
+      </c>
+      <c r="B13" t="s">
+        <v>327</v>
+      </c>
+      <c r="C13" t="s">
+        <v>44</v>
+      </c>
+      <c r="D13" t="s">
+        <v>89</v>
+      </c>
+      <c r="E13" t="s">
+        <v>324</v>
+      </c>
+      <c r="F13" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -3593,7 +3616,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:G52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+    <sheetView topLeftCell="A37" workbookViewId="0">
       <selection activeCell="C54" sqref="C54"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Update JSON keys from "eb" to "be" across instruments
Renamed all occurrences of the key "eb" to "be" for consistency in the `instruments_tree.json` structure. Updated corresponding solution values to reflect this adjustment without altering logic or data integrity.
</commit_message>
<xml_diff>
--- a/Instrument_tree.xlsx
+++ b/Instrument_tree.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Axel\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Axel\PYTHON\FragHub\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6911D80-BAEB-45DB-AE36-ABB0ED53EF96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F089A5F-192D-48F9-AF2E-8CFA9DFFBAA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AB SCIEX" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1842" uniqueCount="325">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1842" uniqueCount="324">
   <si>
     <t>MARQUES</t>
   </si>
@@ -300,9 +300,6 @@
   </si>
   <si>
     <t>JMS-700</t>
-  </si>
-  <si>
-    <t>EB</t>
   </si>
   <si>
     <t>JMS-HX 110</t>
@@ -1946,7 +1943,7 @@
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2615,8 +2612,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2780,7 +2777,7 @@
         <v>8</v>
       </c>
       <c r="D8" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="E8" t="s">
         <v>82</v>
@@ -2794,13 +2791,13 @@
         <v>78</v>
       </c>
       <c r="B9" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C9" t="s">
         <v>8</v>
       </c>
       <c r="D9" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="E9" t="s">
         <v>82</v>
@@ -2814,13 +2811,13 @@
         <v>78</v>
       </c>
       <c r="B10" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C10" t="s">
         <v>8</v>
       </c>
       <c r="D10" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="E10" t="s">
         <v>82</v>
@@ -2834,7 +2831,7 @@
         <v>78</v>
       </c>
       <c r="B11" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C11" t="s">
         <v>8</v>
@@ -2854,7 +2851,7 @@
         <v>78</v>
       </c>
       <c r="B12" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C12" t="s">
         <v>8</v>
@@ -2874,16 +2871,16 @@
         <v>78</v>
       </c>
       <c r="B13" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="C13" t="s">
         <v>46</v>
       </c>
       <c r="D13" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="E13" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="F13" t="s">
         <v>11</v>
@@ -2899,7 +2896,7 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2934,16 +2931,16 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>90</v>
+      </c>
+      <c r="B2" t="s">
         <v>91</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" t="s">
         <v>92</v>
-      </c>
-      <c r="C2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" t="s">
-        <v>93</v>
       </c>
       <c r="E2" t="s">
         <v>10</v>
@@ -2954,10 +2951,10 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C3" t="s">
         <v>46</v>
@@ -2974,10 +2971,10 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C4" t="s">
         <v>46</v>
@@ -2994,10 +2991,10 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C5" t="s">
         <v>46</v>
@@ -3057,10 +3054,10 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>96</v>
+      </c>
+      <c r="B2" t="s">
         <v>97</v>
-      </c>
-      <c r="B2" t="s">
-        <v>98</v>
       </c>
       <c r="C2" t="s">
         <v>8</v>
@@ -3077,10 +3074,10 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C3" t="s">
         <v>8</v>
@@ -3097,10 +3094,10 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C4" t="s">
         <v>8</v>
@@ -3117,10 +3114,10 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C5" t="s">
         <v>8</v>
@@ -3137,10 +3134,10 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C6" t="s">
         <v>8</v>
@@ -3157,10 +3154,10 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B7" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C7" t="s">
         <v>8</v>
@@ -3177,10 +3174,10 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B8" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C8" t="s">
         <v>8</v>
@@ -3197,10 +3194,10 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B9" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C9" t="s">
         <v>8</v>
@@ -3217,10 +3214,10 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B10" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C10" t="s">
         <v>8</v>
@@ -3237,10 +3234,10 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B11" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C11" t="s">
         <v>8</v>
@@ -3257,10 +3254,10 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B12" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C12" t="s">
         <v>8</v>
@@ -3277,10 +3274,10 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B13" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C13" t="s">
         <v>8</v>
@@ -3297,10 +3294,10 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B14" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C14" t="s">
         <v>8</v>
@@ -3317,10 +3314,10 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B15" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C15" t="s">
         <v>8</v>
@@ -3337,10 +3334,10 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B16" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C16" t="s">
         <v>8</v>
@@ -3357,10 +3354,10 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B17" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C17" t="s">
         <v>8</v>
@@ -3377,10 +3374,10 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B18" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C18" t="s">
         <v>8</v>
@@ -3397,10 +3394,10 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B19" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C19" t="s">
         <v>8</v>
@@ -3417,10 +3414,10 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B20" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C20" t="s">
         <v>8</v>
@@ -3437,10 +3434,10 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B21" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C21" t="s">
         <v>8</v>
@@ -3457,10 +3454,10 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B22" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C22" t="s">
         <v>8</v>
@@ -3477,10 +3474,10 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B23" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C23" t="s">
         <v>8</v>
@@ -3497,10 +3494,10 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B24" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C24" t="s">
         <v>8</v>
@@ -3517,10 +3514,10 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B25" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C25" t="s">
         <v>8</v>
@@ -3537,10 +3534,10 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B26" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C26" t="s">
         <v>8</v>
@@ -3557,10 +3554,10 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B27" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C27" t="s">
         <v>8</v>
@@ -3577,10 +3574,10 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B28" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C28" t="s">
         <v>8</v>
@@ -3597,10 +3594,10 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B29" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C29" t="s">
         <v>8</v>
@@ -3624,7 +3621,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:G52"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E47" sqref="E47:E50"/>
     </sheetView>
   </sheetViews>
@@ -3661,10 +3658,10 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>124</v>
+      </c>
+      <c r="B2" t="s">
         <v>125</v>
-      </c>
-      <c r="B2" t="s">
-        <v>126</v>
       </c>
       <c r="C2" t="s">
         <v>8</v>
@@ -3681,10 +3678,10 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C3" t="s">
         <v>8</v>
@@ -3701,10 +3698,10 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C4" t="s">
         <v>8</v>
@@ -3721,10 +3718,10 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C5" t="s">
         <v>8</v>
@@ -3741,10 +3738,10 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B6" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C6" t="s">
         <v>8</v>
@@ -3761,10 +3758,10 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B7" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C7" t="s">
         <v>8</v>
@@ -3781,10 +3778,10 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B8" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C8" t="s">
         <v>8</v>
@@ -3801,10 +3798,10 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B9" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C9" t="s">
         <v>8</v>
@@ -3821,10 +3818,10 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B10" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C10" t="s">
         <v>8</v>
@@ -3841,10 +3838,10 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B11" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C11" t="s">
         <v>8</v>
@@ -3861,10 +3858,10 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B12" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C12" t="s">
         <v>8</v>
@@ -3881,10 +3878,10 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B13" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C13" t="s">
         <v>8</v>
@@ -3901,10 +3898,10 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B14" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C14" t="s">
         <v>8</v>
@@ -3921,10 +3918,10 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B15" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C15" t="s">
         <v>8</v>
@@ -3941,10 +3938,10 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B16" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C16" t="s">
         <v>8</v>
@@ -3961,10 +3958,10 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B17" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C17" t="s">
         <v>8</v>
@@ -3981,10 +3978,10 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B18" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C18" t="s">
         <v>8</v>
@@ -4001,16 +3998,16 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B19" t="s">
+        <v>142</v>
+      </c>
+      <c r="C19" t="s">
+        <v>8</v>
+      </c>
+      <c r="D19" t="s">
         <v>143</v>
-      </c>
-      <c r="C19" t="s">
-        <v>8</v>
-      </c>
-      <c r="D19" t="s">
-        <v>144</v>
       </c>
       <c r="E19" t="s">
         <v>10</v>
@@ -4021,10 +4018,10 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B20" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C20" t="s">
         <v>8</v>
@@ -4041,10 +4038,10 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B21" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C21" t="s">
         <v>8</v>
@@ -4061,16 +4058,16 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B22" t="s">
+        <v>144</v>
+      </c>
+      <c r="C22" t="s">
+        <v>8</v>
+      </c>
+      <c r="D22" t="s">
         <v>145</v>
-      </c>
-      <c r="C22" t="s">
-        <v>8</v>
-      </c>
-      <c r="D22" t="s">
-        <v>146</v>
       </c>
       <c r="E22" t="s">
         <v>10</v>
@@ -4081,16 +4078,16 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B23" t="s">
+        <v>144</v>
+      </c>
+      <c r="C23" t="s">
+        <v>8</v>
+      </c>
+      <c r="D23" t="s">
         <v>145</v>
-      </c>
-      <c r="C23" t="s">
-        <v>8</v>
-      </c>
-      <c r="D23" t="s">
-        <v>146</v>
       </c>
       <c r="E23" t="s">
         <v>35</v>
@@ -4101,16 +4098,16 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B24" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C24" t="s">
         <v>8</v>
       </c>
       <c r="D24" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E24" t="s">
         <v>10</v>
@@ -4121,16 +4118,16 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B25" t="s">
+        <v>147</v>
+      </c>
+      <c r="C25" t="s">
+        <v>8</v>
+      </c>
+      <c r="D25" t="s">
         <v>148</v>
-      </c>
-      <c r="C25" t="s">
-        <v>8</v>
-      </c>
-      <c r="D25" t="s">
-        <v>149</v>
       </c>
       <c r="E25" t="s">
         <v>10</v>
@@ -4141,16 +4138,16 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B26" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C26" t="s">
         <v>8</v>
       </c>
       <c r="D26" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E26" t="s">
         <v>10</v>
@@ -4161,16 +4158,16 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B27" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C27" t="s">
         <v>8</v>
       </c>
       <c r="D27" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E27" t="s">
         <v>10</v>
@@ -4181,10 +4178,10 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B28" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C28" t="s">
         <v>8</v>
@@ -4201,16 +4198,16 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B29" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C29" t="s">
         <v>8</v>
       </c>
       <c r="D29" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E29" t="s">
         <v>10</v>
@@ -4221,16 +4218,16 @@
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B30" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C30" t="s">
         <v>8</v>
       </c>
       <c r="D30" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E30" t="s">
         <v>10</v>
@@ -4241,10 +4238,10 @@
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B31" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C31" t="s">
         <v>8</v>
@@ -4261,16 +4258,16 @@
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B32" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C32" t="s">
         <v>8</v>
       </c>
       <c r="D32" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E32" t="s">
         <v>10</v>
@@ -4281,10 +4278,10 @@
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B33" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C33" t="s">
         <v>8</v>
@@ -4301,16 +4298,16 @@
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B34" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C34" t="s">
         <v>8</v>
       </c>
       <c r="D34" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E34" t="s">
         <v>10</v>
@@ -4321,10 +4318,10 @@
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B35" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C35" t="s">
         <v>8</v>
@@ -4341,16 +4338,16 @@
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B36" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C36" t="s">
         <v>8</v>
       </c>
       <c r="D36" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E36" t="s">
         <v>10</v>
@@ -4361,16 +4358,16 @@
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B37" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C37" t="s">
         <v>8</v>
       </c>
       <c r="D37" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E37" t="s">
         <v>10</v>
@@ -4381,16 +4378,16 @@
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B38" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C38" t="s">
         <v>8</v>
       </c>
       <c r="D38" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E38" t="s">
         <v>35</v>
@@ -4401,16 +4398,16 @@
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B39" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C39" t="s">
         <v>8</v>
       </c>
       <c r="D39" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E39" t="s">
         <v>10</v>
@@ -4421,10 +4418,10 @@
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B40" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C40" t="s">
         <v>8</v>
@@ -4441,10 +4438,10 @@
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B41" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C41" t="s">
         <v>46</v>
@@ -4453,7 +4450,7 @@
         <v>9</v>
       </c>
       <c r="E41" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="F41" t="s">
         <v>11</v>
@@ -4461,10 +4458,10 @@
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B42" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C42" t="s">
         <v>8</v>
@@ -4473,7 +4470,7 @@
         <v>9</v>
       </c>
       <c r="E42" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="F42" t="s">
         <v>11</v>
@@ -4481,10 +4478,10 @@
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B43" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C43" t="s">
         <v>8</v>
@@ -4493,7 +4490,7 @@
         <v>9</v>
       </c>
       <c r="E43" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="F43" t="s">
         <v>11</v>
@@ -4501,10 +4498,10 @@
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B44" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C44" t="s">
         <v>8</v>
@@ -4513,7 +4510,7 @@
         <v>9</v>
       </c>
       <c r="E44" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="F44" t="s">
         <v>11</v>
@@ -4521,10 +4518,10 @@
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B45" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C45" t="s">
         <v>46</v>
@@ -4541,16 +4538,16 @@
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C46" s="2" t="s">
         <v>46</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E46" s="2" t="s">
         <v>35</v>
@@ -4561,19 +4558,19 @@
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C47" s="2" t="s">
         <v>46</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E47" s="4" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="F47" s="2" t="s">
         <v>14</v>
@@ -4581,16 +4578,16 @@
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C48" s="2" t="s">
         <v>46</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E48" s="4" t="s">
         <v>48</v>
@@ -4602,16 +4599,16 @@
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C49" s="2" t="s">
         <v>46</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E49" s="4" t="s">
         <v>35</v>
@@ -4622,19 +4619,19 @@
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C50" s="2" t="s">
         <v>46</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E50" s="4" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="F50" s="2" t="s">
         <v>14</v>
@@ -4642,16 +4639,16 @@
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C51" s="2" t="s">
         <v>46</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E51" s="2" t="s">
         <v>48</v>
@@ -4673,7 +4670,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:F156"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A145" workbookViewId="0">
       <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
@@ -4709,13 +4706,13 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>167</v>
+      </c>
+      <c r="B2" t="s">
         <v>168</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>169</v>
-      </c>
-      <c r="C2" t="s">
-        <v>170</v>
       </c>
       <c r="D2" t="s">
         <v>22</v>
@@ -4729,10 +4726,10 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C3" t="s">
         <v>8</v>
@@ -4749,10 +4746,10 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B4" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C4" t="s">
         <v>8</v>
@@ -4769,10 +4766,10 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B5" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C5" t="s">
         <v>8</v>
@@ -4789,10 +4786,10 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B6" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C6" t="s">
         <v>8</v>
@@ -4809,10 +4806,10 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B7" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C7" t="s">
         <v>8</v>
@@ -4829,10 +4826,10 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B8" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C8" t="s">
         <v>8</v>
@@ -4849,10 +4846,10 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B9" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C9" t="s">
         <v>8</v>
@@ -4869,10 +4866,10 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B10" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C10" t="s">
         <v>8</v>
@@ -4889,10 +4886,10 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B11" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C11" t="s">
         <v>8</v>
@@ -4909,10 +4906,10 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B12" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C12" t="s">
         <v>8</v>
@@ -4929,10 +4926,10 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B13" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C13" t="s">
         <v>8</v>
@@ -4949,10 +4946,10 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B14" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C14" t="s">
         <v>8</v>
@@ -4969,10 +4966,10 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B15" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C15" t="s">
         <v>8</v>
@@ -4989,10 +4986,10 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B16" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C16" t="s">
         <v>8</v>
@@ -5009,10 +5006,10 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B17" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C17" t="s">
         <v>8</v>
@@ -5029,10 +5026,10 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B18" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C18" t="s">
         <v>8</v>
@@ -5049,10 +5046,10 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B19" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C19" t="s">
         <v>8</v>
@@ -5069,10 +5066,10 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B20" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C20" t="s">
         <v>8</v>
@@ -5089,10 +5086,10 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B21" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C21" t="s">
         <v>8</v>
@@ -5109,10 +5106,10 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B22" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C22" t="s">
         <v>8</v>
@@ -5129,10 +5126,10 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B23" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C23" t="s">
         <v>8</v>
@@ -5149,10 +5146,10 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B24" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C24" t="s">
         <v>8</v>
@@ -5169,10 +5166,10 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B25" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C25" t="s">
         <v>8</v>
@@ -5189,10 +5186,10 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B26" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C26" t="s">
         <v>8</v>
@@ -5209,10 +5206,10 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B27" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C27" t="s">
         <v>8</v>
@@ -5229,10 +5226,10 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B28" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C28" t="s">
         <v>8</v>
@@ -5249,10 +5246,10 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B29" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C29" t="s">
         <v>8</v>
@@ -5269,10 +5266,10 @@
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B30" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C30" t="s">
         <v>8</v>
@@ -5289,10 +5286,10 @@
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B31" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C31" t="s">
         <v>8</v>
@@ -5309,10 +5306,10 @@
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B32" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C32" t="s">
         <v>8</v>
@@ -5329,10 +5326,10 @@
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B33" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C33" t="s">
         <v>8</v>
@@ -5349,10 +5346,10 @@
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B34" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C34" t="s">
         <v>8</v>
@@ -5369,10 +5366,10 @@
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B35" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C35" t="s">
         <v>8</v>
@@ -5389,10 +5386,10 @@
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B36" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C36" t="s">
         <v>8</v>
@@ -5409,10 +5406,10 @@
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B37" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C37" t="s">
         <v>8</v>
@@ -5429,10 +5426,10 @@
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B38" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C38" t="s">
         <v>8</v>
@@ -5449,10 +5446,10 @@
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B39" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C39" t="s">
         <v>8</v>
@@ -5469,10 +5466,10 @@
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B40" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C40" t="s">
         <v>8</v>
@@ -5489,10 +5486,10 @@
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B41" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C41" t="s">
         <v>8</v>
@@ -5509,10 +5506,10 @@
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B42" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C42" t="s">
         <v>8</v>
@@ -5529,10 +5526,10 @@
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B43" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C43" t="s">
         <v>8</v>
@@ -5549,10 +5546,10 @@
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B44" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C44" t="s">
         <v>8</v>
@@ -5569,10 +5566,10 @@
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B45" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C45" t="s">
         <v>8</v>
@@ -5589,10 +5586,10 @@
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B46" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C46" t="s">
         <v>8</v>
@@ -5609,10 +5606,10 @@
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B47" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C47" t="s">
         <v>8</v>
@@ -5629,10 +5626,10 @@
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B48" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C48" t="s">
         <v>8</v>
@@ -5649,10 +5646,10 @@
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B49" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C49" t="s">
         <v>8</v>
@@ -5669,10 +5666,10 @@
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B50" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C50" t="s">
         <v>8</v>
@@ -5689,10 +5686,10 @@
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B51" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C51" t="s">
         <v>8</v>
@@ -5709,10 +5706,10 @@
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B52" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C52" t="s">
         <v>8</v>
@@ -5729,10 +5726,10 @@
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B53" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C53" t="s">
         <v>8</v>
@@ -5749,10 +5746,10 @@
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B54" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C54" t="s">
         <v>8</v>
@@ -5769,10 +5766,10 @@
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B55" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C55" t="s">
         <v>8</v>
@@ -5789,10 +5786,10 @@
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B56" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C56" t="s">
         <v>8</v>
@@ -5809,10 +5806,10 @@
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B57" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C57" t="s">
         <v>8</v>
@@ -5829,10 +5826,10 @@
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B58" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C58" t="s">
         <v>8</v>
@@ -5849,10 +5846,10 @@
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B59" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C59" t="s">
         <v>8</v>
@@ -5869,10 +5866,10 @@
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B60" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C60" t="s">
         <v>8</v>
@@ -5889,10 +5886,10 @@
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B61" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C61" t="s">
         <v>8</v>
@@ -5909,10 +5906,10 @@
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B62" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C62" t="s">
         <v>8</v>
@@ -5929,10 +5926,10 @@
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B63" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C63" t="s">
         <v>8</v>
@@ -5949,10 +5946,10 @@
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B64" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C64" t="s">
         <v>8</v>
@@ -5969,10 +5966,10 @@
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B65" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C65" t="s">
         <v>8</v>
@@ -5989,10 +5986,10 @@
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B66" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C66" t="s">
         <v>8</v>
@@ -6009,10 +6006,10 @@
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B67" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C67" t="s">
         <v>8</v>
@@ -6029,10 +6026,10 @@
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B68" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C68" t="s">
         <v>8</v>
@@ -6049,10 +6046,10 @@
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B69" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C69" t="s">
         <v>8</v>
@@ -6069,10 +6066,10 @@
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B70" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C70" t="s">
         <v>8</v>
@@ -6089,10 +6086,10 @@
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B71" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C71" t="s">
         <v>8</v>
@@ -6109,10 +6106,10 @@
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B72" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C72" t="s">
         <v>8</v>
@@ -6129,10 +6126,10 @@
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B73" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C73" t="s">
         <v>8</v>
@@ -6149,10 +6146,10 @@
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B74" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C74" t="s">
         <v>8</v>
@@ -6169,10 +6166,10 @@
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B75" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C75" t="s">
         <v>8</v>
@@ -6189,10 +6186,10 @@
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B76" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C76" t="s">
         <v>8</v>
@@ -6209,10 +6206,10 @@
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B77" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C77" t="s">
         <v>8</v>
@@ -6229,10 +6226,10 @@
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B78" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C78" t="s">
         <v>8</v>
@@ -6249,10 +6246,10 @@
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B79" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C79" t="s">
         <v>8</v>
@@ -6269,10 +6266,10 @@
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B80" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C80" t="s">
         <v>8</v>
@@ -6289,10 +6286,10 @@
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B81" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C81" t="s">
         <v>8</v>
@@ -6309,10 +6306,10 @@
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B82" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C82" t="s">
         <v>8</v>
@@ -6329,10 +6326,10 @@
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B83" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C83" t="s">
         <v>8</v>
@@ -6349,10 +6346,10 @@
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B84" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C84" t="s">
         <v>8</v>
@@ -6369,10 +6366,10 @@
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B85" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C85" t="s">
         <v>8</v>
@@ -6389,10 +6386,10 @@
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B86" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C86" t="s">
         <v>8</v>
@@ -6409,10 +6406,10 @@
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B87" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C87" t="s">
         <v>8</v>
@@ -6429,10 +6426,10 @@
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B88" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C88" t="s">
         <v>8</v>
@@ -6449,10 +6446,10 @@
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B89" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C89" t="s">
         <v>8</v>
@@ -6469,10 +6466,10 @@
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B90" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C90" t="s">
         <v>8</v>
@@ -6489,10 +6486,10 @@
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B91" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C91" t="s">
         <v>8</v>
@@ -6509,10 +6506,10 @@
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B92" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C92" t="s">
         <v>8</v>
@@ -6529,10 +6526,10 @@
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B93" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C93" t="s">
         <v>8</v>
@@ -6549,10 +6546,10 @@
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B94" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C94" t="s">
         <v>8</v>
@@ -6569,10 +6566,10 @@
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B95" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C95" t="s">
         <v>8</v>
@@ -6589,10 +6586,10 @@
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B96" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C96" t="s">
         <v>8</v>
@@ -6609,10 +6606,10 @@
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B97" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C97" t="s">
         <v>8</v>
@@ -6629,10 +6626,10 @@
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B98" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C98" t="s">
         <v>8</v>
@@ -6649,10 +6646,10 @@
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B99" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C99" t="s">
         <v>8</v>
@@ -6669,10 +6666,10 @@
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B100" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C100" t="s">
         <v>8</v>
@@ -6689,10 +6686,10 @@
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B101" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C101" t="s">
         <v>8</v>
@@ -6709,10 +6706,10 @@
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B102" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C102" t="s">
         <v>8</v>
@@ -6729,10 +6726,10 @@
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B103" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C103" t="s">
         <v>8</v>
@@ -6749,10 +6746,10 @@
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B104" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C104" t="s">
         <v>8</v>
@@ -6769,10 +6766,10 @@
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B105" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C105" t="s">
         <v>8</v>
@@ -6789,10 +6786,10 @@
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B106" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C106" t="s">
         <v>8</v>
@@ -6809,10 +6806,10 @@
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B107" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C107" t="s">
         <v>8</v>
@@ -6829,10 +6826,10 @@
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B108" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C108" t="s">
         <v>8</v>
@@ -6849,10 +6846,10 @@
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B109" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C109" t="s">
         <v>8</v>
@@ -6869,10 +6866,10 @@
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B110" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C110" t="s">
         <v>8</v>
@@ -6889,10 +6886,10 @@
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B111" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C111" t="s">
         <v>8</v>
@@ -6909,10 +6906,10 @@
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B112" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C112" t="s">
         <v>8</v>
@@ -6929,10 +6926,10 @@
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B113" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="C113" t="s">
         <v>8</v>
@@ -6949,10 +6946,10 @@
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B114" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="C114" t="s">
         <v>8</v>
@@ -6969,10 +6966,10 @@
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B115" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C115" t="s">
         <v>8</v>
@@ -6989,10 +6986,10 @@
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B116" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C116" t="s">
         <v>8</v>
@@ -7009,10 +7006,10 @@
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B117" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C117" t="s">
         <v>8</v>
@@ -7029,10 +7026,10 @@
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B118" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C118" t="s">
         <v>8</v>
@@ -7049,10 +7046,10 @@
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B119" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C119" t="s">
         <v>8</v>
@@ -7069,10 +7066,10 @@
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B120" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C120" t="s">
         <v>8</v>
@@ -7089,10 +7086,10 @@
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B121" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C121" t="s">
         <v>8</v>
@@ -7109,10 +7106,10 @@
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B122" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C122" t="s">
         <v>8</v>
@@ -7129,10 +7126,10 @@
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B123" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="C123" t="s">
         <v>8</v>
@@ -7149,10 +7146,10 @@
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B124" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C124" t="s">
         <v>8</v>
@@ -7169,10 +7166,10 @@
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B125" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="C125" t="s">
         <v>8</v>
@@ -7189,10 +7186,10 @@
     </row>
     <row r="126" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B126" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C126" t="s">
         <v>8</v>
@@ -7209,10 +7206,10 @@
     </row>
     <row r="127" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B127" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C127" t="s">
         <v>8</v>
@@ -7229,10 +7226,10 @@
     </row>
     <row r="128" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B128" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C128" t="s">
         <v>8</v>
@@ -7249,10 +7246,10 @@
     </row>
     <row r="129" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B129" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C129" t="s">
         <v>8</v>
@@ -7269,10 +7266,10 @@
     </row>
     <row r="130" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B130" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C130" t="s">
         <v>8</v>
@@ -7289,10 +7286,10 @@
     </row>
     <row r="131" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B131" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C131" t="s">
         <v>8</v>
@@ -7309,10 +7306,10 @@
     </row>
     <row r="132" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B132" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C132" t="s">
         <v>8</v>
@@ -7329,10 +7326,10 @@
     </row>
     <row r="133" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B133" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C133" t="s">
         <v>8</v>
@@ -7349,10 +7346,10 @@
     </row>
     <row r="134" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B134" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="C134" t="s">
         <v>8</v>
@@ -7369,10 +7366,10 @@
     </row>
     <row r="135" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B135" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="C135" t="s">
         <v>8</v>
@@ -7389,10 +7386,10 @@
     </row>
     <row r="136" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B136" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C136" t="s">
         <v>8</v>
@@ -7409,10 +7406,10 @@
     </row>
     <row r="137" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B137" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C137" t="s">
         <v>8</v>
@@ -7429,10 +7426,10 @@
     </row>
     <row r="138" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B138" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C138" t="s">
         <v>8</v>
@@ -7449,10 +7446,10 @@
     </row>
     <row r="139" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B139" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C139" t="s">
         <v>8</v>
@@ -7469,10 +7466,10 @@
     </row>
     <row r="140" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B140" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C140" t="s">
         <v>8</v>
@@ -7489,10 +7486,10 @@
     </row>
     <row r="141" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B141" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="C141" t="s">
         <v>8</v>
@@ -7509,10 +7506,10 @@
     </row>
     <row r="142" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B142" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="C142" t="s">
         <v>8</v>
@@ -7529,10 +7526,10 @@
     </row>
     <row r="143" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B143" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="C143" t="s">
         <v>8</v>
@@ -7549,10 +7546,10 @@
     </row>
     <row r="144" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B144" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C144" t="s">
         <v>8</v>
@@ -7569,10 +7566,10 @@
     </row>
     <row r="145" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B145" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C145" t="s">
         <v>8</v>
@@ -7589,10 +7586,10 @@
     </row>
     <row r="146" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B146" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="C146" t="s">
         <v>8</v>
@@ -7609,10 +7606,10 @@
     </row>
     <row r="147" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B147" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="C147" t="s">
         <v>8</v>
@@ -7629,10 +7626,10 @@
     </row>
     <row r="148" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B148" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C148" t="s">
         <v>8</v>
@@ -7649,10 +7646,10 @@
     </row>
     <row r="149" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B149" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="C149" t="s">
         <v>8</v>
@@ -7669,10 +7666,10 @@
     </row>
     <row r="150" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B150" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="C150" t="s">
         <v>8</v>
@@ -7689,10 +7686,10 @@
     </row>
     <row r="151" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B151" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="C151" t="s">
         <v>8</v>
@@ -7709,13 +7706,13 @@
     </row>
     <row r="152" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B152" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="C152" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D152" t="s">
         <v>17</v>
@@ -7729,10 +7726,10 @@
     </row>
     <row r="153" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B153" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="C153" t="s">
         <v>8</v>
@@ -7749,10 +7746,10 @@
     </row>
     <row r="154" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B154" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="C154" t="s">
         <v>8</v>
@@ -7769,16 +7766,16 @@
     </row>
     <row r="155" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B155" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="C155" t="s">
         <v>8</v>
       </c>
       <c r="D155" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E155" t="s">
         <v>10</v>
@@ -7789,10 +7786,10 @@
     </row>
     <row r="156" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B156" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="C156" t="s">
         <v>8</v>

</xml_diff>

<commit_message>
Refactor instrument tree solution mappings and update logic
Revised the handling of `SPECTRUM_TYPE` determination logic by removing redundant `EI` mapping for LC. Updated `instruments_tree.json` to align solution names like `GC-PTR-TOF` by simplifying and standardizing naming conventions. This ensures consistency across solutions and reduces ambiguity in instrument configuration mappings.
</commit_message>
<xml_diff>
--- a/Instrument_tree.xlsx
+++ b/Instrument_tree.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Axel\PYTHON\FragHub\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F089A5F-192D-48F9-AF2E-8CFA9DFFBAA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A692BD63-97C7-4DF4-A792-8EB1DB7A56C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-285" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AB SCIEX" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1842" uniqueCount="324">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1842" uniqueCount="322">
   <si>
     <t>MARQUES</t>
   </si>
@@ -248,21 +248,12 @@
     <t>PTR3</t>
   </si>
   <si>
-    <t>CI-TOF</t>
-  </si>
-  <si>
     <t xml:space="preserve">PTR-QMS 500 </t>
   </si>
   <si>
-    <t>CI-Q</t>
-  </si>
-  <si>
     <t>PTR-TOF 1000</t>
   </si>
   <si>
-    <t>PTR-TOF</t>
-  </si>
-  <si>
     <t>PTR</t>
   </si>
   <si>
@@ -320,9 +311,6 @@
     <t xml:space="preserve">M-4100 </t>
   </si>
   <si>
-    <t>BE</t>
-  </si>
-  <si>
     <t>M-60</t>
   </si>
   <si>
@@ -1014,6 +1002,12 @@
   </si>
   <si>
     <t>JMS-700V</t>
+  </si>
+  <si>
+    <t>EBEB</t>
+  </si>
+  <si>
+    <t>EB</t>
   </si>
 </sst>
 </file>
@@ -2430,7 +2424,7 @@
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2474,7 +2468,7 @@
         <v>46</v>
       </c>
       <c r="D2" t="s">
-        <v>68</v>
+        <v>22</v>
       </c>
       <c r="E2" t="s">
         <v>48</v>
@@ -2488,13 +2482,13 @@
         <v>66</v>
       </c>
       <c r="B3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C3" t="s">
         <v>46</v>
       </c>
       <c r="D3" t="s">
-        <v>70</v>
+        <v>42</v>
       </c>
       <c r="E3" t="s">
         <v>48</v>
@@ -2508,16 +2502,16 @@
         <v>66</v>
       </c>
       <c r="B4" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C4" t="s">
         <v>46</v>
       </c>
       <c r="D4" t="s">
-        <v>72</v>
+        <v>22</v>
       </c>
       <c r="E4" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="F4" t="s">
         <v>11</v>
@@ -2528,16 +2522,16 @@
         <v>66</v>
       </c>
       <c r="B5" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C5" t="s">
         <v>46</v>
       </c>
       <c r="D5" t="s">
-        <v>72</v>
+        <v>22</v>
       </c>
       <c r="E5" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="F5" t="s">
         <v>11</v>
@@ -2548,16 +2542,16 @@
         <v>66</v>
       </c>
       <c r="B6" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C6" t="s">
         <v>46</v>
       </c>
       <c r="D6" t="s">
-        <v>72</v>
+        <v>22</v>
       </c>
       <c r="E6" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="F6" t="s">
         <v>14</v>
@@ -2568,16 +2562,16 @@
         <v>66</v>
       </c>
       <c r="B7" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C7" t="s">
         <v>46</v>
       </c>
       <c r="D7" t="s">
-        <v>72</v>
+        <v>22</v>
       </c>
       <c r="E7" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="F7" t="s">
         <v>14</v>
@@ -2588,16 +2582,16 @@
         <v>66</v>
       </c>
       <c r="B8" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C8" t="s">
         <v>46</v>
       </c>
       <c r="D8" t="s">
-        <v>72</v>
+        <v>22</v>
       </c>
       <c r="E8" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="F8" t="s">
         <v>14</v>
@@ -2613,7 +2607,7 @@
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2648,10 +2642,10 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B2" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C2" t="s">
         <v>46</v>
@@ -2668,10 +2662,10 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B3" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C3" t="s">
         <v>46</v>
@@ -2688,10 +2682,10 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>75</v>
+      </c>
+      <c r="B4" t="s">
         <v>78</v>
-      </c>
-      <c r="B4" t="s">
-        <v>81</v>
       </c>
       <c r="C4" t="s">
         <v>8</v>
@@ -2700,7 +2694,7 @@
         <v>47</v>
       </c>
       <c r="E4" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="F4" t="s">
         <v>11</v>
@@ -2708,10 +2702,10 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>75</v>
+      </c>
+      <c r="B5" t="s">
         <v>78</v>
-      </c>
-      <c r="B5" t="s">
-        <v>81</v>
       </c>
       <c r="C5" t="s">
         <v>8</v>
@@ -2720,7 +2714,7 @@
         <v>47</v>
       </c>
       <c r="E5" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="F5" t="s">
         <v>11</v>
@@ -2728,10 +2722,10 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>75</v>
+      </c>
+      <c r="B6" t="s">
         <v>78</v>
-      </c>
-      <c r="B6" t="s">
-        <v>81</v>
       </c>
       <c r="C6" t="s">
         <v>46</v>
@@ -2748,10 +2742,10 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B7" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C7" t="s">
         <v>8</v>
@@ -2760,7 +2754,7 @@
         <v>47</v>
       </c>
       <c r="E7" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="F7" t="s">
         <v>11</v>
@@ -2768,19 +2762,19 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B8" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C8" t="s">
         <v>8</v>
       </c>
       <c r="D8" t="s">
-        <v>92</v>
+        <v>321</v>
       </c>
       <c r="E8" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="F8" t="s">
         <v>11</v>
@@ -2788,19 +2782,19 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B9" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C9" t="s">
         <v>8</v>
       </c>
       <c r="D9" t="s">
-        <v>92</v>
+        <v>321</v>
       </c>
       <c r="E9" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="F9" t="s">
         <v>11</v>
@@ -2808,19 +2802,19 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B10" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C10" t="s">
         <v>8</v>
       </c>
       <c r="D10" t="s">
-        <v>92</v>
+        <v>320</v>
       </c>
       <c r="E10" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="F10" t="s">
         <v>11</v>
@@ -2828,10 +2822,10 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B11" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C11" t="s">
         <v>8</v>
@@ -2848,10 +2842,10 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B12" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C12" t="s">
         <v>8</v>
@@ -2868,19 +2862,19 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B13" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
       <c r="C13" t="s">
         <v>46</v>
       </c>
       <c r="D13" t="s">
-        <v>92</v>
+        <v>321</v>
       </c>
       <c r="E13" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="F13" t="s">
         <v>11</v>
@@ -2896,7 +2890,7 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2931,16 +2925,16 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B2" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="C2" t="s">
         <v>8</v>
       </c>
       <c r="D2" t="s">
-        <v>92</v>
+        <v>321</v>
       </c>
       <c r="E2" t="s">
         <v>10</v>
@@ -2951,10 +2945,10 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B3" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="C3" t="s">
         <v>46</v>
@@ -2971,10 +2965,10 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>87</v>
+      </c>
+      <c r="B4" t="s">
         <v>90</v>
-      </c>
-      <c r="B4" t="s">
-        <v>94</v>
       </c>
       <c r="C4" t="s">
         <v>46</v>
@@ -2991,10 +2985,10 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B5" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="C5" t="s">
         <v>46</v>
@@ -3054,10 +3048,10 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="B2" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="C2" t="s">
         <v>8</v>
@@ -3074,10 +3068,10 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="B3" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="C3" t="s">
         <v>8</v>
@@ -3094,10 +3088,10 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="B4" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="C4" t="s">
         <v>8</v>
@@ -3114,10 +3108,10 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>92</v>
+      </c>
+      <c r="B5" t="s">
         <v>96</v>
-      </c>
-      <c r="B5" t="s">
-        <v>100</v>
       </c>
       <c r="C5" t="s">
         <v>8</v>
@@ -3134,10 +3128,10 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="B6" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="C6" t="s">
         <v>8</v>
@@ -3154,10 +3148,10 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="B7" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="C7" t="s">
         <v>8</v>
@@ -3174,10 +3168,10 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="B8" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="C8" t="s">
         <v>8</v>
@@ -3194,10 +3188,10 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="B9" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="C9" t="s">
         <v>8</v>
@@ -3214,10 +3208,10 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="B10" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="C10" t="s">
         <v>8</v>
@@ -3234,10 +3228,10 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="B11" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="C11" t="s">
         <v>8</v>
@@ -3254,10 +3248,10 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="B12" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C12" t="s">
         <v>8</v>
@@ -3274,10 +3268,10 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="B13" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="C13" t="s">
         <v>8</v>
@@ -3294,10 +3288,10 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="B14" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="C14" t="s">
         <v>8</v>
@@ -3314,10 +3308,10 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="B15" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="C15" t="s">
         <v>8</v>
@@ -3334,10 +3328,10 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="B16" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="C16" t="s">
         <v>8</v>
@@ -3354,10 +3348,10 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="B17" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="C17" t="s">
         <v>8</v>
@@ -3374,10 +3368,10 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="B18" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="C18" t="s">
         <v>8</v>
@@ -3394,10 +3388,10 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="B19" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="C19" t="s">
         <v>8</v>
@@ -3414,10 +3408,10 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="B20" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="C20" t="s">
         <v>8</v>
@@ -3434,10 +3428,10 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="B21" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="C21" t="s">
         <v>8</v>
@@ -3454,10 +3448,10 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="B22" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="C22" t="s">
         <v>8</v>
@@ -3474,10 +3468,10 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="B23" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="C23" t="s">
         <v>8</v>
@@ -3494,10 +3488,10 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="B24" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="C24" t="s">
         <v>8</v>
@@ -3514,10 +3508,10 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="B25" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="C25" t="s">
         <v>8</v>
@@ -3534,10 +3528,10 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="B26" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="C26" t="s">
         <v>8</v>
@@ -3554,10 +3548,10 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="B27" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="C27" t="s">
         <v>8</v>
@@ -3574,10 +3568,10 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="B28" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="C28" t="s">
         <v>8</v>
@@ -3594,10 +3588,10 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="B29" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="C29" t="s">
         <v>8</v>
@@ -3621,7 +3615,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:G52"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="E47" sqref="E47:E50"/>
     </sheetView>
   </sheetViews>
@@ -3658,10 +3652,10 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="B2" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="C2" t="s">
         <v>8</v>
@@ -3678,10 +3672,10 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="B3" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="C3" t="s">
         <v>8</v>
@@ -3698,10 +3692,10 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="B4" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="C4" t="s">
         <v>8</v>
@@ -3718,10 +3712,10 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>120</v>
+      </c>
+      <c r="B5" t="s">
         <v>124</v>
-      </c>
-      <c r="B5" t="s">
-        <v>128</v>
       </c>
       <c r="C5" t="s">
         <v>8</v>
@@ -3738,10 +3732,10 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="B6" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="C6" t="s">
         <v>8</v>
@@ -3758,10 +3752,10 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="B7" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="C7" t="s">
         <v>8</v>
@@ -3778,10 +3772,10 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="B8" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="C8" t="s">
         <v>8</v>
@@ -3798,10 +3792,10 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="B9" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="C9" t="s">
         <v>8</v>
@@ -3818,10 +3812,10 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="B10" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="C10" t="s">
         <v>8</v>
@@ -3838,10 +3832,10 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="B11" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="C11" t="s">
         <v>8</v>
@@ -3858,10 +3852,10 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="B12" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="C12" t="s">
         <v>8</v>
@@ -3878,10 +3872,10 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="B13" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="C13" t="s">
         <v>8</v>
@@ -3898,10 +3892,10 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="B14" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="C14" t="s">
         <v>8</v>
@@ -3918,10 +3912,10 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="B15" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="C15" t="s">
         <v>8</v>
@@ -3938,10 +3932,10 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="B16" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="C16" t="s">
         <v>8</v>
@@ -3958,10 +3952,10 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="B17" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="C17" t="s">
         <v>8</v>
@@ -3978,10 +3972,10 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="B18" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="C18" t="s">
         <v>8</v>
@@ -3998,16 +3992,16 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="B19" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="C19" t="s">
         <v>8</v>
       </c>
       <c r="D19" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="E19" t="s">
         <v>10</v>
@@ -4018,10 +4012,10 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="B20" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="C20" t="s">
         <v>8</v>
@@ -4038,10 +4032,10 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="B21" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="C21" t="s">
         <v>8</v>
@@ -4058,16 +4052,16 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="B22" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="C22" t="s">
         <v>8</v>
       </c>
       <c r="D22" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="E22" t="s">
         <v>10</v>
@@ -4078,16 +4072,16 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="B23" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="C23" t="s">
         <v>8</v>
       </c>
       <c r="D23" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="E23" t="s">
         <v>35</v>
@@ -4098,16 +4092,16 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="B24" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="C24" t="s">
         <v>8</v>
       </c>
       <c r="D24" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="E24" t="s">
         <v>10</v>
@@ -4118,16 +4112,16 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="B25" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="C25" t="s">
         <v>8</v>
       </c>
       <c r="D25" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="E25" t="s">
         <v>10</v>
@@ -4138,16 +4132,16 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="B26" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="C26" t="s">
         <v>8</v>
       </c>
       <c r="D26" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="E26" t="s">
         <v>10</v>
@@ -4158,16 +4152,16 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="B27" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="C27" t="s">
         <v>8</v>
       </c>
       <c r="D27" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="E27" t="s">
         <v>10</v>
@@ -4178,10 +4172,10 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="B28" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="C28" t="s">
         <v>8</v>
@@ -4198,16 +4192,16 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="B29" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="C29" t="s">
         <v>8</v>
       </c>
       <c r="D29" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="E29" t="s">
         <v>10</v>
@@ -4218,16 +4212,16 @@
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="B30" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="C30" t="s">
         <v>8</v>
       </c>
       <c r="D30" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="E30" t="s">
         <v>10</v>
@@ -4238,10 +4232,10 @@
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="B31" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="C31" t="s">
         <v>8</v>
@@ -4258,16 +4252,16 @@
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="B32" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="C32" t="s">
         <v>8</v>
       </c>
       <c r="D32" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="E32" t="s">
         <v>10</v>
@@ -4278,10 +4272,10 @@
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="B33" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="C33" t="s">
         <v>8</v>
@@ -4298,16 +4292,16 @@
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="B34" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="C34" t="s">
         <v>8</v>
       </c>
       <c r="D34" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="E34" t="s">
         <v>10</v>
@@ -4318,10 +4312,10 @@
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="B35" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="C35" t="s">
         <v>8</v>
@@ -4338,16 +4332,16 @@
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="B36" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="C36" t="s">
         <v>8</v>
       </c>
       <c r="D36" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="E36" t="s">
         <v>10</v>
@@ -4358,16 +4352,16 @@
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="B37" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="C37" t="s">
         <v>8</v>
       </c>
       <c r="D37" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="E37" t="s">
         <v>10</v>
@@ -4378,16 +4372,16 @@
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="B38" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="C38" t="s">
         <v>8</v>
       </c>
       <c r="D38" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="E38" t="s">
         <v>35</v>
@@ -4398,16 +4392,16 @@
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="B39" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="C39" t="s">
         <v>8</v>
       </c>
       <c r="D39" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="E39" t="s">
         <v>10</v>
@@ -4418,10 +4412,10 @@
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="B40" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="C40" t="s">
         <v>8</v>
@@ -4438,10 +4432,10 @@
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="B41" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="C41" t="s">
         <v>46</v>
@@ -4450,7 +4444,7 @@
         <v>9</v>
       </c>
       <c r="E41" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="F41" t="s">
         <v>11</v>
@@ -4458,10 +4452,10 @@
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="B42" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="C42" t="s">
         <v>8</v>
@@ -4470,7 +4464,7 @@
         <v>9</v>
       </c>
       <c r="E42" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="F42" t="s">
         <v>11</v>
@@ -4478,10 +4472,10 @@
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="B43" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="C43" t="s">
         <v>8</v>
@@ -4490,7 +4484,7 @@
         <v>9</v>
       </c>
       <c r="E43" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="F43" t="s">
         <v>11</v>
@@ -4498,10 +4492,10 @@
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="B44" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="C44" t="s">
         <v>8</v>
@@ -4510,7 +4504,7 @@
         <v>9</v>
       </c>
       <c r="E44" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="F44" t="s">
         <v>11</v>
@@ -4518,10 +4512,10 @@
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="B45" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="C45" t="s">
         <v>46</v>
@@ -4538,16 +4532,16 @@
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="C46" s="2" t="s">
         <v>46</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="E46" s="2" t="s">
         <v>35</v>
@@ -4558,19 +4552,19 @@
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="C47" s="2" t="s">
         <v>46</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="E47" s="4" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="F47" s="2" t="s">
         <v>14</v>
@@ -4578,16 +4572,16 @@
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="C48" s="2" t="s">
         <v>46</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="E48" s="4" t="s">
         <v>48</v>
@@ -4599,16 +4593,16 @@
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="C49" s="2" t="s">
         <v>46</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="E49" s="4" t="s">
         <v>35</v>
@@ -4619,19 +4613,19 @@
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="C50" s="2" t="s">
         <v>46</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="E50" s="4" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="F50" s="2" t="s">
         <v>14</v>
@@ -4639,16 +4633,16 @@
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="C51" s="2" t="s">
         <v>46</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="E51" s="2" t="s">
         <v>48</v>
@@ -4670,7 +4664,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:F156"/>
   <sheetViews>
-    <sheetView topLeftCell="A145" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
@@ -4706,13 +4700,13 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="B2" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="C2" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="D2" t="s">
         <v>22</v>
@@ -4726,10 +4720,10 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="B3" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="C3" t="s">
         <v>8</v>
@@ -4746,10 +4740,10 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>163</v>
+      </c>
+      <c r="B4" t="s">
         <v>167</v>
-      </c>
-      <c r="B4" t="s">
-        <v>171</v>
       </c>
       <c r="C4" t="s">
         <v>8</v>
@@ -4766,10 +4760,10 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="B5" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="C5" t="s">
         <v>8</v>
@@ -4786,10 +4780,10 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="B6" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="C6" t="s">
         <v>8</v>
@@ -4806,10 +4800,10 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="B7" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="C7" t="s">
         <v>8</v>
@@ -4826,10 +4820,10 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="B8" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="C8" t="s">
         <v>8</v>
@@ -4846,10 +4840,10 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="B9" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="C9" t="s">
         <v>8</v>
@@ -4866,10 +4860,10 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="B10" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="C10" t="s">
         <v>8</v>
@@ -4886,10 +4880,10 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="B11" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="C11" t="s">
         <v>8</v>
@@ -4906,10 +4900,10 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="B12" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="C12" t="s">
         <v>8</v>
@@ -4926,10 +4920,10 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="B13" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="C13" t="s">
         <v>8</v>
@@ -4946,10 +4940,10 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="B14" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="C14" t="s">
         <v>8</v>
@@ -4966,10 +4960,10 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="B15" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="C15" t="s">
         <v>8</v>
@@ -4986,10 +4980,10 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="B16" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="C16" t="s">
         <v>8</v>
@@ -5006,10 +5000,10 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="B17" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="C17" t="s">
         <v>8</v>
@@ -5026,10 +5020,10 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="B18" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="C18" t="s">
         <v>8</v>
@@ -5046,10 +5040,10 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="B19" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="C19" t="s">
         <v>8</v>
@@ -5066,10 +5060,10 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="B20" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="C20" t="s">
         <v>8</v>
@@ -5086,10 +5080,10 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="B21" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="C21" t="s">
         <v>8</v>
@@ -5106,10 +5100,10 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="B22" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="C22" t="s">
         <v>8</v>
@@ -5126,10 +5120,10 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="B23" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="C23" t="s">
         <v>8</v>
@@ -5146,10 +5140,10 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="B24" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="C24" t="s">
         <v>8</v>
@@ -5166,10 +5160,10 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="B25" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="C25" t="s">
         <v>8</v>
@@ -5186,10 +5180,10 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="B26" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="C26" t="s">
         <v>8</v>
@@ -5206,10 +5200,10 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="B27" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="C27" t="s">
         <v>8</v>
@@ -5226,10 +5220,10 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="B28" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="C28" t="s">
         <v>8</v>
@@ -5246,10 +5240,10 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="B29" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="C29" t="s">
         <v>8</v>
@@ -5266,10 +5260,10 @@
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="B30" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="C30" t="s">
         <v>8</v>
@@ -5286,10 +5280,10 @@
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="B31" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="C31" t="s">
         <v>8</v>
@@ -5306,10 +5300,10 @@
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="B32" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="C32" t="s">
         <v>8</v>
@@ -5326,10 +5320,10 @@
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="B33" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="C33" t="s">
         <v>8</v>
@@ -5346,10 +5340,10 @@
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="B34" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="C34" t="s">
         <v>8</v>
@@ -5366,10 +5360,10 @@
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="B35" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="C35" t="s">
         <v>8</v>
@@ -5386,10 +5380,10 @@
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="B36" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="C36" t="s">
         <v>8</v>
@@ -5406,10 +5400,10 @@
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="B37" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="C37" t="s">
         <v>8</v>
@@ -5426,10 +5420,10 @@
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="B38" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="C38" t="s">
         <v>8</v>
@@ -5446,10 +5440,10 @@
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="B39" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="C39" t="s">
         <v>8</v>
@@ -5466,10 +5460,10 @@
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="B40" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="C40" t="s">
         <v>8</v>
@@ -5486,10 +5480,10 @@
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="B41" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="C41" t="s">
         <v>8</v>
@@ -5506,10 +5500,10 @@
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="B42" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="C42" t="s">
         <v>8</v>
@@ -5526,10 +5520,10 @@
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="B43" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="C43" t="s">
         <v>8</v>
@@ -5546,10 +5540,10 @@
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="B44" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="C44" t="s">
         <v>8</v>
@@ -5566,10 +5560,10 @@
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="B45" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="C45" t="s">
         <v>8</v>
@@ -5586,10 +5580,10 @@
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="B46" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="C46" t="s">
         <v>8</v>
@@ -5606,10 +5600,10 @@
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="B47" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="C47" t="s">
         <v>8</v>
@@ -5626,10 +5620,10 @@
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="B48" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="C48" t="s">
         <v>8</v>
@@ -5646,10 +5640,10 @@
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="B49" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="C49" t="s">
         <v>8</v>
@@ -5666,10 +5660,10 @@
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="B50" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="C50" t="s">
         <v>8</v>
@@ -5686,10 +5680,10 @@
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="B51" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="C51" t="s">
         <v>8</v>
@@ -5706,10 +5700,10 @@
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="B52" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="C52" t="s">
         <v>8</v>
@@ -5726,10 +5720,10 @@
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="B53" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="C53" t="s">
         <v>8</v>
@@ -5746,10 +5740,10 @@
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="B54" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="C54" t="s">
         <v>8</v>
@@ -5766,10 +5760,10 @@
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="B55" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="C55" t="s">
         <v>8</v>
@@ -5786,10 +5780,10 @@
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="B56" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="C56" t="s">
         <v>8</v>
@@ -5806,10 +5800,10 @@
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="B57" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="C57" t="s">
         <v>8</v>
@@ -5826,10 +5820,10 @@
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="B58" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="C58" t="s">
         <v>8</v>
@@ -5846,10 +5840,10 @@
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="B59" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="C59" t="s">
         <v>8</v>
@@ -5866,10 +5860,10 @@
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="B60" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="C60" t="s">
         <v>8</v>
@@ -5886,10 +5880,10 @@
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="B61" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="C61" t="s">
         <v>8</v>
@@ -5906,10 +5900,10 @@
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="B62" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="C62" t="s">
         <v>8</v>
@@ -5926,10 +5920,10 @@
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="B63" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="C63" t="s">
         <v>8</v>
@@ -5946,10 +5940,10 @@
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="B64" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="C64" t="s">
         <v>8</v>
@@ -5966,10 +5960,10 @@
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="B65" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="C65" t="s">
         <v>8</v>
@@ -5986,10 +5980,10 @@
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="B66" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="C66" t="s">
         <v>8</v>
@@ -6006,10 +6000,10 @@
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="B67" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="C67" t="s">
         <v>8</v>
@@ -6026,10 +6020,10 @@
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="B68" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="C68" t="s">
         <v>8</v>
@@ -6046,10 +6040,10 @@
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="B69" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="C69" t="s">
         <v>8</v>
@@ -6066,10 +6060,10 @@
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="B70" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="C70" t="s">
         <v>8</v>
@@ -6086,10 +6080,10 @@
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="B71" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="C71" t="s">
         <v>8</v>
@@ -6106,10 +6100,10 @@
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="B72" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="C72" t="s">
         <v>8</v>
@@ -6126,10 +6120,10 @@
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="B73" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="C73" t="s">
         <v>8</v>
@@ -6146,10 +6140,10 @@
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="B74" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="C74" t="s">
         <v>8</v>
@@ -6166,10 +6160,10 @@
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="B75" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="C75" t="s">
         <v>8</v>
@@ -6186,10 +6180,10 @@
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="B76" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="C76" t="s">
         <v>8</v>
@@ -6206,10 +6200,10 @@
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="B77" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="C77" t="s">
         <v>8</v>
@@ -6226,10 +6220,10 @@
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="B78" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="C78" t="s">
         <v>8</v>
@@ -6246,10 +6240,10 @@
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="B79" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="C79" t="s">
         <v>8</v>
@@ -6266,10 +6260,10 @@
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="B80" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="C80" t="s">
         <v>8</v>
@@ -6286,10 +6280,10 @@
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="B81" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="C81" t="s">
         <v>8</v>
@@ -6306,10 +6300,10 @@
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="B82" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="C82" t="s">
         <v>8</v>
@@ -6326,10 +6320,10 @@
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="B83" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="C83" t="s">
         <v>8</v>
@@ -6346,10 +6340,10 @@
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="B84" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="C84" t="s">
         <v>8</v>
@@ -6366,10 +6360,10 @@
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="B85" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="C85" t="s">
         <v>8</v>
@@ -6386,10 +6380,10 @@
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="B86" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="C86" t="s">
         <v>8</v>
@@ -6406,10 +6400,10 @@
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="B87" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="C87" t="s">
         <v>8</v>
@@ -6426,10 +6420,10 @@
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="B88" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="C88" t="s">
         <v>8</v>
@@ -6446,10 +6440,10 @@
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="B89" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="C89" t="s">
         <v>8</v>
@@ -6466,10 +6460,10 @@
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="B90" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="C90" t="s">
         <v>8</v>
@@ -6486,10 +6480,10 @@
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="B91" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="C91" t="s">
         <v>8</v>
@@ -6506,10 +6500,10 @@
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="B92" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="C92" t="s">
         <v>8</v>
@@ -6526,10 +6520,10 @@
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="B93" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="C93" t="s">
         <v>8</v>
@@ -6546,10 +6540,10 @@
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="B94" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="C94" t="s">
         <v>8</v>
@@ -6566,10 +6560,10 @@
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="B95" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="C95" t="s">
         <v>8</v>
@@ -6586,10 +6580,10 @@
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="B96" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="C96" t="s">
         <v>8</v>
@@ -6606,10 +6600,10 @@
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="B97" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="C97" t="s">
         <v>8</v>
@@ -6626,10 +6620,10 @@
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="B98" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="C98" t="s">
         <v>8</v>
@@ -6646,10 +6640,10 @@
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="B99" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="C99" t="s">
         <v>8</v>
@@ -6666,10 +6660,10 @@
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="B100" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="C100" t="s">
         <v>8</v>
@@ -6686,10 +6680,10 @@
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="B101" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="C101" t="s">
         <v>8</v>
@@ -6706,10 +6700,10 @@
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="B102" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="C102" t="s">
         <v>8</v>
@@ -6726,10 +6720,10 @@
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="B103" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="C103" t="s">
         <v>8</v>
@@ -6746,10 +6740,10 @@
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="B104" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="C104" t="s">
         <v>8</v>
@@ -6766,10 +6760,10 @@
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="B105" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="C105" t="s">
         <v>8</v>
@@ -6786,10 +6780,10 @@
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="B106" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="C106" t="s">
         <v>8</v>
@@ -6806,10 +6800,10 @@
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="B107" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="C107" t="s">
         <v>8</v>
@@ -6826,10 +6820,10 @@
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="B108" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="C108" t="s">
         <v>8</v>
@@ -6846,10 +6840,10 @@
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="B109" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="C109" t="s">
         <v>8</v>
@@ -6866,10 +6860,10 @@
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="B110" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="C110" t="s">
         <v>8</v>
@@ -6886,10 +6880,10 @@
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="B111" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="C111" t="s">
         <v>8</v>
@@ -6906,10 +6900,10 @@
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="B112" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="C112" t="s">
         <v>8</v>
@@ -6926,10 +6920,10 @@
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="B113" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="C113" t="s">
         <v>8</v>
@@ -6946,10 +6940,10 @@
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="B114" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="C114" t="s">
         <v>8</v>
@@ -6966,10 +6960,10 @@
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="B115" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
       <c r="C115" t="s">
         <v>8</v>
@@ -6986,10 +6980,10 @@
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="B116" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="C116" t="s">
         <v>8</v>
@@ -7006,10 +7000,10 @@
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="B117" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="C117" t="s">
         <v>8</v>
@@ -7026,10 +7020,10 @@
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="B118" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="C118" t="s">
         <v>8</v>
@@ -7046,10 +7040,10 @@
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="B119" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="C119" t="s">
         <v>8</v>
@@ -7066,10 +7060,10 @@
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="B120" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="C120" t="s">
         <v>8</v>
@@ -7086,10 +7080,10 @@
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="B121" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="C121" t="s">
         <v>8</v>
@@ -7106,10 +7100,10 @@
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="B122" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
       <c r="C122" t="s">
         <v>8</v>
@@ -7126,10 +7120,10 @@
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="B123" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="C123" t="s">
         <v>8</v>
@@ -7146,10 +7140,10 @@
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="B124" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="C124" t="s">
         <v>8</v>
@@ -7166,10 +7160,10 @@
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="B125" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="C125" t="s">
         <v>8</v>
@@ -7186,10 +7180,10 @@
     </row>
     <row r="126" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="B126" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="C126" t="s">
         <v>8</v>
@@ -7206,10 +7200,10 @@
     </row>
     <row r="127" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="B127" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="C127" t="s">
         <v>8</v>
@@ -7226,10 +7220,10 @@
     </row>
     <row r="128" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="B128" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="C128" t="s">
         <v>8</v>
@@ -7246,10 +7240,10 @@
     </row>
     <row r="129" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="B129" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="C129" t="s">
         <v>8</v>
@@ -7266,10 +7260,10 @@
     </row>
     <row r="130" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="B130" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="C130" t="s">
         <v>8</v>
@@ -7286,10 +7280,10 @@
     </row>
     <row r="131" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="B131" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="C131" t="s">
         <v>8</v>
@@ -7306,10 +7300,10 @@
     </row>
     <row r="132" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="B132" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="C132" t="s">
         <v>8</v>
@@ -7326,10 +7320,10 @@
     </row>
     <row r="133" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="B133" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="C133" t="s">
         <v>8</v>
@@ -7346,10 +7340,10 @@
     </row>
     <row r="134" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="B134" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
       <c r="C134" t="s">
         <v>8</v>
@@ -7366,10 +7360,10 @@
     </row>
     <row r="135" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="B135" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
       <c r="C135" t="s">
         <v>8</v>
@@ -7386,10 +7380,10 @@
     </row>
     <row r="136" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="B136" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
       <c r="C136" t="s">
         <v>8</v>
@@ -7406,10 +7400,10 @@
     </row>
     <row r="137" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="B137" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
       <c r="C137" t="s">
         <v>8</v>
@@ -7426,10 +7420,10 @@
     </row>
     <row r="138" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="B138" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="C138" t="s">
         <v>8</v>
@@ -7446,10 +7440,10 @@
     </row>
     <row r="139" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="B139" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
       <c r="C139" t="s">
         <v>8</v>
@@ -7466,10 +7460,10 @@
     </row>
     <row r="140" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="B140" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="C140" t="s">
         <v>8</v>
@@ -7486,10 +7480,10 @@
     </row>
     <row r="141" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="B141" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="C141" t="s">
         <v>8</v>
@@ -7506,10 +7500,10 @@
     </row>
     <row r="142" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="B142" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="C142" t="s">
         <v>8</v>
@@ -7526,10 +7520,10 @@
     </row>
     <row r="143" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="B143" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
       <c r="C143" t="s">
         <v>8</v>
@@ -7546,10 +7540,10 @@
     </row>
     <row r="144" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="B144" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
       <c r="C144" t="s">
         <v>8</v>
@@ -7566,10 +7560,10 @@
     </row>
     <row r="145" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="B145" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="C145" t="s">
         <v>8</v>
@@ -7586,10 +7580,10 @@
     </row>
     <row r="146" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="B146" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
       <c r="C146" t="s">
         <v>8</v>
@@ -7606,10 +7600,10 @@
     </row>
     <row r="147" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="B147" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="C147" t="s">
         <v>8</v>
@@ -7626,10 +7620,10 @@
     </row>
     <row r="148" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="B148" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
       <c r="C148" t="s">
         <v>8</v>
@@ -7646,10 +7640,10 @@
     </row>
     <row r="149" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="B149" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="C149" t="s">
         <v>8</v>
@@ -7666,10 +7660,10 @@
     </row>
     <row r="150" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="B150" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="C150" t="s">
         <v>8</v>
@@ -7686,10 +7680,10 @@
     </row>
     <row r="151" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="B151" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
       <c r="C151" t="s">
         <v>8</v>
@@ -7706,13 +7700,13 @@
     </row>
     <row r="152" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="B152" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
       <c r="C152" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="D152" t="s">
         <v>17</v>
@@ -7726,10 +7720,10 @@
     </row>
     <row r="153" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="B153" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="C153" t="s">
         <v>8</v>
@@ -7746,10 +7740,10 @@
     </row>
     <row r="154" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="B154" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="C154" t="s">
         <v>8</v>
@@ -7766,16 +7760,16 @@
     </row>
     <row r="155" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="B155" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
       <c r="C155" t="s">
         <v>8</v>
       </c>
       <c r="D155" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="E155" t="s">
         <v>10</v>
@@ -7786,10 +7780,10 @@
     </row>
     <row r="156" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="B156" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
       <c r="C156" t="s">
         <v>8</v>

</xml_diff>

<commit_message>
Restructure and update instrument configurations in JSON.
Reordered and added missing configurations for various instruments to ensure consistency and correctness. Reintroduced missing keys, refined the hierarchy, and streamlined data structures to better align with other entries.
</commit_message>
<xml_diff>
--- a/Instrument_tree.xlsx
+++ b/Instrument_tree.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Axel\PYTHON\FragHub\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A692BD63-97C7-4DF4-A792-8EB1DB7A56C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D714BA6-08C8-443D-8F69-C91E15EB75AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-285" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AB SCIEX" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1842" uniqueCount="322">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1848" uniqueCount="322">
   <si>
     <t>MARQUES</t>
   </si>
@@ -2604,10 +2604,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L12" sqref="L12"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2825,19 +2825,19 @@
         <v>75</v>
       </c>
       <c r="B11" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C11" t="s">
-        <v>8</v>
+        <v>46</v>
       </c>
       <c r="D11" t="s">
-        <v>22</v>
+        <v>320</v>
       </c>
       <c r="E11" t="s">
-        <v>38</v>
+        <v>156</v>
       </c>
       <c r="F11" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -2845,7 +2845,7 @@
         <v>75</v>
       </c>
       <c r="B12" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C12" t="s">
         <v>8</v>
@@ -2854,7 +2854,7 @@
         <v>22</v>
       </c>
       <c r="E12" t="s">
-        <v>10</v>
+        <v>38</v>
       </c>
       <c r="F12" t="s">
         <v>14</v>
@@ -2865,18 +2865,38 @@
         <v>75</v>
       </c>
       <c r="B13" t="s">
+        <v>86</v>
+      </c>
+      <c r="C13" t="s">
+        <v>8</v>
+      </c>
+      <c r="D13" t="s">
+        <v>22</v>
+      </c>
+      <c r="E13" t="s">
+        <v>10</v>
+      </c>
+      <c r="F13" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>75</v>
+      </c>
+      <c r="B14" t="s">
         <v>319</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C14" t="s">
         <v>46</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D14" t="s">
         <v>321</v>
       </c>
-      <c r="E13" t="s">
+      <c r="E14" t="s">
         <v>156</v>
       </c>
-      <c r="F13" t="s">
+      <c r="F14" t="s">
         <v>11</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fix and reorganize instrument mappings in instruments_tree.json
Reorganized and corrected nested structure for instrument models, including Agilent MSD 1100, 6210, 6544, 6560, and G2445A. Readded some entries such as 6544 and 6560 while fixing inconsistencies in mappings for LC, QIT, QTOF, ESI, and TOF configurations. Improved clarity and accuracy of the instrument classification hierarchy.
</commit_message>
<xml_diff>
--- a/Instrument_tree.xlsx
+++ b/Instrument_tree.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Axel\PYTHON\FragHub\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D714BA6-08C8-443D-8F69-C91E15EB75AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6349F7A3-53C4-4350-AF5D-171651E5F29B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AB SCIEX" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1848" uniqueCount="322">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1854" uniqueCount="322">
   <si>
     <t>MARQUES</t>
   </si>
@@ -2606,7 +2606,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:F14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
@@ -4682,10 +4682,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <dimension ref="A1:F156"/>
+  <dimension ref="A1:F157"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4726,7 +4726,7 @@
         <v>164</v>
       </c>
       <c r="C2" t="s">
-        <v>165</v>
+        <v>8</v>
       </c>
       <c r="D2" t="s">
         <v>22</v>
@@ -4743,19 +4743,19 @@
         <v>163</v>
       </c>
       <c r="B3" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C3" t="s">
-        <v>8</v>
+        <v>165</v>
       </c>
       <c r="D3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="E3" t="s">
         <v>10</v>
       </c>
       <c r="F3" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -4763,19 +4763,19 @@
         <v>163</v>
       </c>
       <c r="B4" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C4" t="s">
         <v>8</v>
       </c>
       <c r="D4" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="E4" t="s">
         <v>10</v>
       </c>
       <c r="F4" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -4783,7 +4783,7 @@
         <v>163</v>
       </c>
       <c r="B5" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C5" t="s">
         <v>8</v>
@@ -4803,7 +4803,7 @@
         <v>163</v>
       </c>
       <c r="B6" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C6" t="s">
         <v>8</v>
@@ -4823,7 +4823,7 @@
         <v>163</v>
       </c>
       <c r="B7" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C7" t="s">
         <v>8</v>
@@ -4843,7 +4843,7 @@
         <v>163</v>
       </c>
       <c r="B8" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C8" t="s">
         <v>8</v>
@@ -4863,7 +4863,7 @@
         <v>163</v>
       </c>
       <c r="B9" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C9" t="s">
         <v>8</v>
@@ -4883,7 +4883,7 @@
         <v>163</v>
       </c>
       <c r="B10" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C10" t="s">
         <v>8</v>
@@ -4903,7 +4903,7 @@
         <v>163</v>
       </c>
       <c r="B11" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C11" t="s">
         <v>8</v>
@@ -4923,7 +4923,7 @@
         <v>163</v>
       </c>
       <c r="B12" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C12" t="s">
         <v>8</v>
@@ -4943,7 +4943,7 @@
         <v>163</v>
       </c>
       <c r="B13" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C13" t="s">
         <v>8</v>
@@ -4963,7 +4963,7 @@
         <v>163</v>
       </c>
       <c r="B14" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C14" t="s">
         <v>8</v>
@@ -4983,7 +4983,7 @@
         <v>163</v>
       </c>
       <c r="B15" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C15" t="s">
         <v>8</v>
@@ -5003,7 +5003,7 @@
         <v>163</v>
       </c>
       <c r="B16" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C16" t="s">
         <v>8</v>
@@ -5023,7 +5023,7 @@
         <v>163</v>
       </c>
       <c r="B17" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C17" t="s">
         <v>8</v>
@@ -5043,7 +5043,7 @@
         <v>163</v>
       </c>
       <c r="B18" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C18" t="s">
         <v>8</v>
@@ -5063,7 +5063,7 @@
         <v>163</v>
       </c>
       <c r="B19" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C19" t="s">
         <v>8</v>
@@ -5083,7 +5083,7 @@
         <v>163</v>
       </c>
       <c r="B20" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C20" t="s">
         <v>8</v>
@@ -5103,7 +5103,7 @@
         <v>163</v>
       </c>
       <c r="B21" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C21" t="s">
         <v>8</v>
@@ -5123,7 +5123,7 @@
         <v>163</v>
       </c>
       <c r="B22" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C22" t="s">
         <v>8</v>
@@ -5143,7 +5143,7 @@
         <v>163</v>
       </c>
       <c r="B23" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C23" t="s">
         <v>8</v>
@@ -5163,7 +5163,7 @@
         <v>163</v>
       </c>
       <c r="B24" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C24" t="s">
         <v>8</v>
@@ -5183,7 +5183,7 @@
         <v>163</v>
       </c>
       <c r="B25" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C25" t="s">
         <v>8</v>
@@ -5203,7 +5203,7 @@
         <v>163</v>
       </c>
       <c r="B26" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C26" t="s">
         <v>8</v>
@@ -5223,7 +5223,7 @@
         <v>163</v>
       </c>
       <c r="B27" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C27" t="s">
         <v>8</v>
@@ -5243,7 +5243,7 @@
         <v>163</v>
       </c>
       <c r="B28" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C28" t="s">
         <v>8</v>
@@ -5263,7 +5263,7 @@
         <v>163</v>
       </c>
       <c r="B29" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C29" t="s">
         <v>8</v>
@@ -5283,7 +5283,7 @@
         <v>163</v>
       </c>
       <c r="B30" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C30" t="s">
         <v>8</v>
@@ -5303,7 +5303,7 @@
         <v>163</v>
       </c>
       <c r="B31" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C31" t="s">
         <v>8</v>
@@ -5323,7 +5323,7 @@
         <v>163</v>
       </c>
       <c r="B32" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C32" t="s">
         <v>8</v>
@@ -5343,7 +5343,7 @@
         <v>163</v>
       </c>
       <c r="B33" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C33" t="s">
         <v>8</v>
@@ -5363,7 +5363,7 @@
         <v>163</v>
       </c>
       <c r="B34" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C34" t="s">
         <v>8</v>
@@ -5383,7 +5383,7 @@
         <v>163</v>
       </c>
       <c r="B35" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C35" t="s">
         <v>8</v>
@@ -5403,7 +5403,7 @@
         <v>163</v>
       </c>
       <c r="B36" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C36" t="s">
         <v>8</v>
@@ -5423,7 +5423,7 @@
         <v>163</v>
       </c>
       <c r="B37" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C37" t="s">
         <v>8</v>
@@ -5443,7 +5443,7 @@
         <v>163</v>
       </c>
       <c r="B38" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C38" t="s">
         <v>8</v>
@@ -5463,7 +5463,7 @@
         <v>163</v>
       </c>
       <c r="B39" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C39" t="s">
         <v>8</v>
@@ -5483,7 +5483,7 @@
         <v>163</v>
       </c>
       <c r="B40" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C40" t="s">
         <v>8</v>
@@ -5503,7 +5503,7 @@
         <v>163</v>
       </c>
       <c r="B41" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C41" t="s">
         <v>8</v>
@@ -5523,7 +5523,7 @@
         <v>163</v>
       </c>
       <c r="B42" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C42" t="s">
         <v>8</v>
@@ -5543,7 +5543,7 @@
         <v>163</v>
       </c>
       <c r="B43" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C43" t="s">
         <v>8</v>
@@ -5563,7 +5563,7 @@
         <v>163</v>
       </c>
       <c r="B44" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C44" t="s">
         <v>8</v>
@@ -5583,7 +5583,7 @@
         <v>163</v>
       </c>
       <c r="B45" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C45" t="s">
         <v>8</v>
@@ -5603,7 +5603,7 @@
         <v>163</v>
       </c>
       <c r="B46" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C46" t="s">
         <v>8</v>
@@ -5623,7 +5623,7 @@
         <v>163</v>
       </c>
       <c r="B47" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C47" t="s">
         <v>8</v>
@@ -5643,7 +5643,7 @@
         <v>163</v>
       </c>
       <c r="B48" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C48" t="s">
         <v>8</v>
@@ -5663,7 +5663,7 @@
         <v>163</v>
       </c>
       <c r="B49" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C49" t="s">
         <v>8</v>
@@ -5683,7 +5683,7 @@
         <v>163</v>
       </c>
       <c r="B50" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C50" t="s">
         <v>8</v>
@@ -5703,7 +5703,7 @@
         <v>163</v>
       </c>
       <c r="B51" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C51" t="s">
         <v>8</v>
@@ -5723,7 +5723,7 @@
         <v>163</v>
       </c>
       <c r="B52" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C52" t="s">
         <v>8</v>
@@ -5743,7 +5743,7 @@
         <v>163</v>
       </c>
       <c r="B53" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C53" t="s">
         <v>8</v>
@@ -5763,7 +5763,7 @@
         <v>163</v>
       </c>
       <c r="B54" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C54" t="s">
         <v>8</v>
@@ -5783,7 +5783,7 @@
         <v>163</v>
       </c>
       <c r="B55" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C55" t="s">
         <v>8</v>
@@ -5803,7 +5803,7 @@
         <v>163</v>
       </c>
       <c r="B56" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C56" t="s">
         <v>8</v>
@@ -5823,7 +5823,7 @@
         <v>163</v>
       </c>
       <c r="B57" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C57" t="s">
         <v>8</v>
@@ -5843,7 +5843,7 @@
         <v>163</v>
       </c>
       <c r="B58" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C58" t="s">
         <v>8</v>
@@ -5863,7 +5863,7 @@
         <v>163</v>
       </c>
       <c r="B59" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C59" t="s">
         <v>8</v>
@@ -5883,7 +5883,7 @@
         <v>163</v>
       </c>
       <c r="B60" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C60" t="s">
         <v>8</v>
@@ -5903,7 +5903,7 @@
         <v>163</v>
       </c>
       <c r="B61" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C61" t="s">
         <v>8</v>
@@ -5923,7 +5923,7 @@
         <v>163</v>
       </c>
       <c r="B62" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C62" t="s">
         <v>8</v>
@@ -5943,7 +5943,7 @@
         <v>163</v>
       </c>
       <c r="B63" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C63" t="s">
         <v>8</v>
@@ -5963,7 +5963,7 @@
         <v>163</v>
       </c>
       <c r="B64" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C64" t="s">
         <v>8</v>
@@ -5983,7 +5983,7 @@
         <v>163</v>
       </c>
       <c r="B65" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C65" t="s">
         <v>8</v>
@@ -6003,7 +6003,7 @@
         <v>163</v>
       </c>
       <c r="B66" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C66" t="s">
         <v>8</v>
@@ -6023,7 +6023,7 @@
         <v>163</v>
       </c>
       <c r="B67" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C67" t="s">
         <v>8</v>
@@ -6043,7 +6043,7 @@
         <v>163</v>
       </c>
       <c r="B68" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C68" t="s">
         <v>8</v>
@@ -6063,7 +6063,7 @@
         <v>163</v>
       </c>
       <c r="B69" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C69" t="s">
         <v>8</v>
@@ -6083,7 +6083,7 @@
         <v>163</v>
       </c>
       <c r="B70" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C70" t="s">
         <v>8</v>
@@ -6103,7 +6103,7 @@
         <v>163</v>
       </c>
       <c r="B71" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C71" t="s">
         <v>8</v>
@@ -6123,7 +6123,7 @@
         <v>163</v>
       </c>
       <c r="B72" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C72" t="s">
         <v>8</v>
@@ -6143,7 +6143,7 @@
         <v>163</v>
       </c>
       <c r="B73" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C73" t="s">
         <v>8</v>
@@ -6163,7 +6163,7 @@
         <v>163</v>
       </c>
       <c r="B74" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C74" t="s">
         <v>8</v>
@@ -6183,7 +6183,7 @@
         <v>163</v>
       </c>
       <c r="B75" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C75" t="s">
         <v>8</v>
@@ -6203,7 +6203,7 @@
         <v>163</v>
       </c>
       <c r="B76" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C76" t="s">
         <v>8</v>
@@ -6223,7 +6223,7 @@
         <v>163</v>
       </c>
       <c r="B77" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C77" t="s">
         <v>8</v>
@@ -6243,7 +6243,7 @@
         <v>163</v>
       </c>
       <c r="B78" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C78" t="s">
         <v>8</v>
@@ -6263,7 +6263,7 @@
         <v>163</v>
       </c>
       <c r="B79" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C79" t="s">
         <v>8</v>
@@ -6283,7 +6283,7 @@
         <v>163</v>
       </c>
       <c r="B80" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C80" t="s">
         <v>8</v>
@@ -6303,7 +6303,7 @@
         <v>163</v>
       </c>
       <c r="B81" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C81" t="s">
         <v>8</v>
@@ -6323,7 +6323,7 @@
         <v>163</v>
       </c>
       <c r="B82" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C82" t="s">
         <v>8</v>
@@ -6343,7 +6343,7 @@
         <v>163</v>
       </c>
       <c r="B83" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C83" t="s">
         <v>8</v>
@@ -6363,7 +6363,7 @@
         <v>163</v>
       </c>
       <c r="B84" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C84" t="s">
         <v>8</v>
@@ -6383,7 +6383,7 @@
         <v>163</v>
       </c>
       <c r="B85" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C85" t="s">
         <v>8</v>
@@ -6403,7 +6403,7 @@
         <v>163</v>
       </c>
       <c r="B86" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C86" t="s">
         <v>8</v>
@@ -6423,7 +6423,7 @@
         <v>163</v>
       </c>
       <c r="B87" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C87" t="s">
         <v>8</v>
@@ -6443,7 +6443,7 @@
         <v>163</v>
       </c>
       <c r="B88" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C88" t="s">
         <v>8</v>
@@ -6463,7 +6463,7 @@
         <v>163</v>
       </c>
       <c r="B89" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C89" t="s">
         <v>8</v>
@@ -6483,7 +6483,7 @@
         <v>163</v>
       </c>
       <c r="B90" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C90" t="s">
         <v>8</v>
@@ -6503,7 +6503,7 @@
         <v>163</v>
       </c>
       <c r="B91" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C91" t="s">
         <v>8</v>
@@ -6523,7 +6523,7 @@
         <v>163</v>
       </c>
       <c r="B92" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C92" t="s">
         <v>8</v>
@@ -6543,7 +6543,7 @@
         <v>163</v>
       </c>
       <c r="B93" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C93" t="s">
         <v>8</v>
@@ -6563,7 +6563,7 @@
         <v>163</v>
       </c>
       <c r="B94" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C94" t="s">
         <v>8</v>
@@ -6583,7 +6583,7 @@
         <v>163</v>
       </c>
       <c r="B95" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C95" t="s">
         <v>8</v>
@@ -6603,7 +6603,7 @@
         <v>163</v>
       </c>
       <c r="B96" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C96" t="s">
         <v>8</v>
@@ -6623,7 +6623,7 @@
         <v>163</v>
       </c>
       <c r="B97" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C97" t="s">
         <v>8</v>
@@ -6643,7 +6643,7 @@
         <v>163</v>
       </c>
       <c r="B98" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C98" t="s">
         <v>8</v>
@@ -6663,7 +6663,7 @@
         <v>163</v>
       </c>
       <c r="B99" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C99" t="s">
         <v>8</v>
@@ -6683,7 +6683,7 @@
         <v>163</v>
       </c>
       <c r="B100" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C100" t="s">
         <v>8</v>
@@ -6703,7 +6703,7 @@
         <v>163</v>
       </c>
       <c r="B101" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C101" t="s">
         <v>8</v>
@@ -6723,7 +6723,7 @@
         <v>163</v>
       </c>
       <c r="B102" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C102" t="s">
         <v>8</v>
@@ -6743,7 +6743,7 @@
         <v>163</v>
       </c>
       <c r="B103" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C103" t="s">
         <v>8</v>
@@ -6763,7 +6763,7 @@
         <v>163</v>
       </c>
       <c r="B104" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C104" t="s">
         <v>8</v>
@@ -6783,7 +6783,7 @@
         <v>163</v>
       </c>
       <c r="B105" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C105" t="s">
         <v>8</v>
@@ -6803,7 +6803,7 @@
         <v>163</v>
       </c>
       <c r="B106" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C106" t="s">
         <v>8</v>
@@ -6823,7 +6823,7 @@
         <v>163</v>
       </c>
       <c r="B107" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C107" t="s">
         <v>8</v>
@@ -6843,7 +6843,7 @@
         <v>163</v>
       </c>
       <c r="B108" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C108" t="s">
         <v>8</v>
@@ -6863,7 +6863,7 @@
         <v>163</v>
       </c>
       <c r="B109" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C109" t="s">
         <v>8</v>
@@ -6883,7 +6883,7 @@
         <v>163</v>
       </c>
       <c r="B110" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C110" t="s">
         <v>8</v>
@@ -6903,7 +6903,7 @@
         <v>163</v>
       </c>
       <c r="B111" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C111" t="s">
         <v>8</v>
@@ -6923,7 +6923,7 @@
         <v>163</v>
       </c>
       <c r="B112" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C112" t="s">
         <v>8</v>
@@ -6943,7 +6943,7 @@
         <v>163</v>
       </c>
       <c r="B113" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C113" t="s">
         <v>8</v>
@@ -6963,7 +6963,7 @@
         <v>163</v>
       </c>
       <c r="B114" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C114" t="s">
         <v>8</v>
@@ -6983,7 +6983,7 @@
         <v>163</v>
       </c>
       <c r="B115" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C115" t="s">
         <v>8</v>
@@ -7003,7 +7003,7 @@
         <v>163</v>
       </c>
       <c r="B116" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C116" t="s">
         <v>8</v>
@@ -7023,7 +7023,7 @@
         <v>163</v>
       </c>
       <c r="B117" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C117" t="s">
         <v>8</v>
@@ -7043,7 +7043,7 @@
         <v>163</v>
       </c>
       <c r="B118" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="C118" t="s">
         <v>8</v>
@@ -7063,7 +7063,7 @@
         <v>163</v>
       </c>
       <c r="B119" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="C119" t="s">
         <v>8</v>
@@ -7083,7 +7083,7 @@
         <v>163</v>
       </c>
       <c r="B120" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C120" t="s">
         <v>8</v>
@@ -7103,7 +7103,7 @@
         <v>163</v>
       </c>
       <c r="B121" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C121" t="s">
         <v>8</v>
@@ -7123,7 +7123,7 @@
         <v>163</v>
       </c>
       <c r="B122" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C122" t="s">
         <v>8</v>
@@ -7143,7 +7143,7 @@
         <v>163</v>
       </c>
       <c r="B123" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C123" t="s">
         <v>8</v>
@@ -7163,7 +7163,7 @@
         <v>163</v>
       </c>
       <c r="B124" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C124" t="s">
         <v>8</v>
@@ -7183,7 +7183,7 @@
         <v>163</v>
       </c>
       <c r="B125" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C125" t="s">
         <v>8</v>
@@ -7203,7 +7203,7 @@
         <v>163</v>
       </c>
       <c r="B126" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C126" t="s">
         <v>8</v>
@@ -7223,7 +7223,7 @@
         <v>163</v>
       </c>
       <c r="B127" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C127" t="s">
         <v>8</v>
@@ -7243,7 +7243,7 @@
         <v>163</v>
       </c>
       <c r="B128" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="C128" t="s">
         <v>8</v>
@@ -7263,7 +7263,7 @@
         <v>163</v>
       </c>
       <c r="B129" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C129" t="s">
         <v>8</v>
@@ -7283,7 +7283,7 @@
         <v>163</v>
       </c>
       <c r="B130" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="C130" t="s">
         <v>8</v>
@@ -7303,7 +7303,7 @@
         <v>163</v>
       </c>
       <c r="B131" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C131" t="s">
         <v>8</v>
@@ -7323,7 +7323,7 @@
         <v>163</v>
       </c>
       <c r="B132" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C132" t="s">
         <v>8</v>
@@ -7343,7 +7343,7 @@
         <v>163</v>
       </c>
       <c r="B133" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C133" t="s">
         <v>8</v>
@@ -7363,7 +7363,7 @@
         <v>163</v>
       </c>
       <c r="B134" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C134" t="s">
         <v>8</v>
@@ -7383,7 +7383,7 @@
         <v>163</v>
       </c>
       <c r="B135" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C135" t="s">
         <v>8</v>
@@ -7403,7 +7403,7 @@
         <v>163</v>
       </c>
       <c r="B136" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C136" t="s">
         <v>8</v>
@@ -7423,7 +7423,7 @@
         <v>163</v>
       </c>
       <c r="B137" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C137" t="s">
         <v>8</v>
@@ -7443,7 +7443,7 @@
         <v>163</v>
       </c>
       <c r="B138" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C138" t="s">
         <v>8</v>
@@ -7463,7 +7463,7 @@
         <v>163</v>
       </c>
       <c r="B139" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="C139" t="s">
         <v>8</v>
@@ -7483,7 +7483,7 @@
         <v>163</v>
       </c>
       <c r="B140" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="C140" t="s">
         <v>8</v>
@@ -7503,7 +7503,7 @@
         <v>163</v>
       </c>
       <c r="B141" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C141" t="s">
         <v>8</v>
@@ -7523,7 +7523,7 @@
         <v>163</v>
       </c>
       <c r="B142" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C142" t="s">
         <v>8</v>
@@ -7543,7 +7543,7 @@
         <v>163</v>
       </c>
       <c r="B143" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C143" t="s">
         <v>8</v>
@@ -7563,7 +7563,7 @@
         <v>163</v>
       </c>
       <c r="B144" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C144" t="s">
         <v>8</v>
@@ -7583,7 +7583,7 @@
         <v>163</v>
       </c>
       <c r="B145" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C145" t="s">
         <v>8</v>
@@ -7603,7 +7603,7 @@
         <v>163</v>
       </c>
       <c r="B146" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="C146" t="s">
         <v>8</v>
@@ -7623,7 +7623,7 @@
         <v>163</v>
       </c>
       <c r="B147" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="C147" t="s">
         <v>8</v>
@@ -7643,7 +7643,7 @@
         <v>163</v>
       </c>
       <c r="B148" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="C148" t="s">
         <v>8</v>
@@ -7663,7 +7663,7 @@
         <v>163</v>
       </c>
       <c r="B149" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C149" t="s">
         <v>8</v>
@@ -7683,7 +7683,7 @@
         <v>163</v>
       </c>
       <c r="B150" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C150" t="s">
         <v>8</v>
@@ -7703,7 +7703,7 @@
         <v>163</v>
       </c>
       <c r="B151" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="C151" t="s">
         <v>8</v>
@@ -7723,10 +7723,10 @@
         <v>163</v>
       </c>
       <c r="B152" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="C152" t="s">
-        <v>165</v>
+        <v>8</v>
       </c>
       <c r="D152" t="s">
         <v>17</v>
@@ -7743,19 +7743,19 @@
         <v>163</v>
       </c>
       <c r="B153" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C153" t="s">
-        <v>8</v>
+        <v>165</v>
       </c>
       <c r="D153" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="E153" t="s">
         <v>10</v>
       </c>
       <c r="F153" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
     </row>
     <row r="154" spans="1:6" x14ac:dyDescent="0.25">
@@ -7763,7 +7763,7 @@
         <v>163</v>
       </c>
       <c r="B154" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="C154" t="s">
         <v>8</v>
@@ -7783,13 +7783,13 @@
         <v>163</v>
       </c>
       <c r="B155" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="C155" t="s">
         <v>8</v>
       </c>
       <c r="D155" t="s">
-        <v>139</v>
+        <v>13</v>
       </c>
       <c r="E155" t="s">
         <v>10</v>
@@ -7809,7 +7809,7 @@
         <v>8</v>
       </c>
       <c r="D156" t="s">
-        <v>13</v>
+        <v>139</v>
       </c>
       <c r="E156" t="s">
         <v>10</v>
@@ -7818,8 +7818,28 @@
         <v>11</v>
       </c>
     </row>
+    <row r="157" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A157" t="s">
+        <v>163</v>
+      </c>
+      <c r="B157" t="s">
+        <v>318</v>
+      </c>
+      <c r="C157" t="s">
+        <v>8</v>
+      </c>
+      <c r="D157" t="s">
+        <v>13</v>
+      </c>
+      <c r="E157" t="s">
+        <v>10</v>
+      </c>
+      <c r="F157" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="A1:F2791">
+  <conditionalFormatting sqref="A1:F2792">
     <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="UNKNOWN">
       <formula>NOT(ISERROR(SEARCH("UNKNOWN",A1)))</formula>
     </cfRule>

</xml_diff>